<commit_message>
- Various modifications to picklists - Various modifications to tableSchema - New UUID code for records - Solved link to analyticalResuluts from AggregatedData (for old reports) - Solved bug of duplicate progId - Added feature for cloning rows (works for each level) - New visualisation of the errors in the browser - Added button for beta testing the Accepted DWH function - Other small changes and bugs fixed
</commit_message>
<xml_diff>
--- a/config/PredefinedResults.xlsx
+++ b/config/PredefinedResults.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="143">
   <si>
     <t>sampAnAsses</t>
   </si>
@@ -601,38 +601,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -1075,6 +1043,38 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -1337,34 +1337,34 @@
   <tableColumns count="10">
     <tableColumn id="1" name="recordType" dataDxfId="23"/>
     <tableColumn id="9" name="source" dataDxfId="22"/>
-    <tableColumn id="10" name="sourceLabel" dataDxfId="0"/>
-    <tableColumn id="6" name="confirmatoryExecuted" dataDxfId="21"/>
-    <tableColumn id="2" name="sampAnAsses" dataDxfId="20"/>
-    <tableColumn id="3" name="sampAnAssesLabel" dataDxfId="19"/>
-    <tableColumn id="4" name="screening" dataDxfId="18"/>
-    <tableColumn id="8" name="confirmatory" dataDxfId="17"/>
-    <tableColumn id="5" name="discriminatory" dataDxfId="16"/>
-    <tableColumn id="7" name="genotypingBaseTerm" dataDxfId="15"/>
+    <tableColumn id="10" name="sourceLabel" dataDxfId="21"/>
+    <tableColumn id="6" name="confirmatoryExecuted" dataDxfId="20"/>
+    <tableColumn id="2" name="sampAnAsses" dataDxfId="19"/>
+    <tableColumn id="3" name="sampAnAssesLabel" dataDxfId="18"/>
+    <tableColumn id="4" name="screening" dataDxfId="17"/>
+    <tableColumn id="8" name="confirmatory" dataDxfId="16"/>
+    <tableColumn id="5" name="discriminatory" dataDxfId="15"/>
+    <tableColumn id="7" name="genotypingBaseTerm" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I29" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I29" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A1:I29"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="recordType" dataDxfId="9"/>
-    <tableColumn id="2" name="anMethtype" dataDxfId="8"/>
-    <tableColumn id="7" name="filter" dataDxfId="7">
+    <tableColumn id="1" name="recordType" dataDxfId="8"/>
+    <tableColumn id="2" name="anMethtype" dataDxfId="7"/>
+    <tableColumn id="7" name="filter" dataDxfId="6">
       <calculatedColumnFormula>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="possible results" dataDxfId="6"/>
-    <tableColumn id="6" name="paramCode" dataDxfId="5"/>
-    <tableColumn id="4" name="param desc" dataDxfId="4"/>
-    <tableColumn id="5" name="resVal" dataDxfId="3"/>
-    <tableColumn id="8" name="codes" dataDxfId="2"/>
-    <tableColumn id="9" name="codici" dataDxfId="1"/>
+    <tableColumn id="3" name="possible results" dataDxfId="5"/>
+    <tableColumn id="6" name="paramCode" dataDxfId="4"/>
+    <tableColumn id="4" name="param desc" dataDxfId="3"/>
+    <tableColumn id="5" name="resVal" dataDxfId="2"/>
+    <tableColumn id="8" name="codes" dataDxfId="1"/>
+    <tableColumn id="9" name="codici" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1660,10 +1660,10 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1983,9 +1983,7 @@
       <c r="H12" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="I12" s="8" t="s">
-        <v>110</v>
-      </c>
+      <c r="I12" s="8"/>
       <c r="J12" s="1" t="s">
         <v>93</v>
       </c>
@@ -2171,9 +2169,7 @@
       <c r="H18" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="I18" s="8" t="s">
-        <v>110</v>
-      </c>
+      <c r="I18" s="8"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added export to excel function for summarized information level
</commit_message>
<xml_diff>
--- a/config/PredefinedResults.xlsx
+++ b/config/PredefinedResults.xlsx
@@ -1,26 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_workspace\tse_workspace\tse-data-reporting-tool\config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CA7480-EB0C-41CD-8AEA-40EEEA9CB16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="resultsLists" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="resultsLists" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" url="C:\Users\monguma\Desktop\resultsLists.xml" htmlTables="1"/>
   </connection>
-  <connection id="2" name="resultsLists1" type="4" refreshedVersion="0" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="resultsLists1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" url="C:\Users\monguma\Desktop\resultsLists.xml" htmlTables="1"/>
   </connection>
 </connections>
@@ -461,7 +478,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -488,6 +505,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1273,6 +1291,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1332,39 +1353,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J45" totalsRowShown="0" dataDxfId="24">
-  <autoFilter ref="A1:J45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J45" totalsRowShown="0" dataDxfId="24">
+  <autoFilter ref="A1:J45" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="recordType" dataDxfId="23"/>
-    <tableColumn id="9" name="source" dataDxfId="22"/>
-    <tableColumn id="10" name="sourceLabel" dataDxfId="21"/>
-    <tableColumn id="6" name="confirmatoryExecuted" dataDxfId="20"/>
-    <tableColumn id="2" name="sampAnAsses" dataDxfId="19"/>
-    <tableColumn id="3" name="sampAnAssesLabel" dataDxfId="18"/>
-    <tableColumn id="4" name="screening" dataDxfId="17"/>
-    <tableColumn id="8" name="confirmatory" dataDxfId="16"/>
-    <tableColumn id="5" name="discriminatory" dataDxfId="15"/>
-    <tableColumn id="7" name="genotypingBaseTerm" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="recordType" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="source" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="sourceLabel" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="confirmatoryExecuted" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="sampAnAsses" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="sampAnAssesLabel" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="screening" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="confirmatory" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="discriminatory" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="genotypingBaseTerm" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I29" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:I29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:I29" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:I29" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="recordType" dataDxfId="8"/>
-    <tableColumn id="2" name="anMethtype" dataDxfId="7"/>
-    <tableColumn id="7" name="filter" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="recordType" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="anMethtype" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="filter" dataDxfId="6">
       <calculatedColumnFormula>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="possible results" dataDxfId="5"/>
-    <tableColumn id="6" name="paramCode" dataDxfId="4"/>
-    <tableColumn id="4" name="param desc" dataDxfId="3"/>
-    <tableColumn id="5" name="resVal" dataDxfId="2"/>
-    <tableColumn id="8" name="codes" dataDxfId="1"/>
-    <tableColumn id="9" name="codici" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="possible results" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="paramCode" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="param desc" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="resVal" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="codes" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="codici" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1413,7 +1434,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1446,9 +1467,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1481,6 +1519,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1656,29 +1711,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomRight" activeCell="G28" sqref="G28:G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="5.21875" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1710,7 +1767,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1736,7 +1793,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1762,7 +1819,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1788,7 +1845,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1814,7 +1871,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1838,7 +1895,7 @@
       <c r="I6" s="15"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1862,7 +1919,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1886,7 +1943,7 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1910,7 +1967,7 @@
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1934,7 +1991,7 @@
       </c>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1958,7 +2015,7 @@
       </c>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1988,7 +2045,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2020,7 +2077,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -2052,7 +2109,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2084,7 +2141,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2116,7 +2173,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2144,7 +2201,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -2172,7 +2229,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -2202,7 +2259,7 @@
       </c>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -2232,7 +2289,7 @@
       </c>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
@@ -2262,7 +2319,7 @@
       </c>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -2292,7 +2349,7 @@
       </c>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -2320,7 +2377,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -2350,7 +2407,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2380,7 +2437,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
@@ -2410,7 +2467,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -2440,7 +2497,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -2470,7 +2527,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
@@ -2492,13 +2549,13 @@
       <c r="G29" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="H29" s="15"/>
+      <c r="H29" s="8"/>
       <c r="I29" s="15" t="s">
         <v>103</v>
       </c>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -2526,7 +2583,7 @@
       </c>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -2554,7 +2611,7 @@
       </c>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
@@ -2582,7 +2639,7 @@
       </c>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
@@ -2610,7 +2667,7 @@
       </c>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>13</v>
       </c>
@@ -2638,7 +2695,7 @@
       </c>
       <c r="J34" s="8"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
@@ -2666,7 +2723,7 @@
       </c>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
@@ -2692,7 +2749,7 @@
       </c>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
@@ -2718,7 +2775,7 @@
       </c>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>19</v>
       </c>
@@ -2744,7 +2801,7 @@
       </c>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>19</v>
       </c>
@@ -2768,7 +2825,7 @@
       <c r="I39" s="15"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
@@ -2792,7 +2849,7 @@
       </c>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>19</v>
       </c>
@@ -2816,7 +2873,7 @@
       </c>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>19</v>
       </c>
@@ -2840,7 +2897,7 @@
       </c>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>19</v>
       </c>
@@ -2864,7 +2921,7 @@
       </c>
       <c r="J43" s="7"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>135</v>
       </c>
@@ -2882,7 +2939,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>135</v>
       </c>
@@ -2909,26 +2966,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="28.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -2957,7 +3014,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2987,7 +3044,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3017,7 +3074,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -3047,7 +3104,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -3077,7 +3134,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -3107,7 +3164,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -3137,7 +3194,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -3167,7 +3224,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -3197,7 +3254,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -3227,7 +3284,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -3257,7 +3314,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -3287,7 +3344,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -3317,7 +3374,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -3347,7 +3404,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -3377,7 +3434,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -3407,7 +3464,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -3437,7 +3494,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -3467,7 +3524,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -3497,7 +3554,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -3527,7 +3584,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -3557,7 +3614,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -3587,7 +3644,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
@@ -3617,7 +3674,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
@@ -3647,7 +3704,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
@@ -3677,7 +3734,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -3707,7 +3764,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
@@ -3737,7 +3794,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>19</v>
       </c>
@@ -3767,7 +3824,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>19</v>
       </c>
@@ -3807,20 +3864,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -3828,7 +3885,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -3836,7 +3893,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -3844,7 +3901,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -3852,7 +3909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -3860,7 +3917,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -3868,7 +3925,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -3876,7 +3933,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -3884,7 +3941,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -3892,7 +3949,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -3900,7 +3957,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -3908,7 +3965,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -3916,7 +3973,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -3924,7 +3981,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -3932,7 +3989,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -3940,7 +3997,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>101</v>
       </c>

</xml_diff>